<commit_message>
Improvements and new examples
Make Android work without Xalan (use stax instead)
Remove usage of thread locals in AlternativeProperty (use references instead)
Show how to get streaming behavior with iterator and how to stream XML.
Pass xml instruction via XML instead of tag metadata.
</commit_message>
<xml_diff>
--- a/Intermediate/HtmlToExcel/result.xlsx
+++ b/Intermediate/HtmlToExcel/result.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339235A3-10FE-4506-8AC5-AC1A708B5E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="30810" yWindow="0" windowWidth="21105" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Colors" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +17,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t/>
+  </si>
   <si>
     <r>
       <rPr>
@@ -56,8 +60,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,12 +86,42 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,8 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -116,6 +155,18 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -124,20 +175,16 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -184,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +263,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,36 +508,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A7D44E-B27A-4FA4-876B-8D3292A078FF}">
+  <dimension ref="B3:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:5" ht="66.75" customHeight="1">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -462,10 +548,10 @@
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -475,24 +561,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CDC8DC-2560-4E49-9D52-B1682BDDB54D}">
+  <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD569A5-52CA-47CD-A82F-B16C97517555}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>